<commit_message>
Update database to include EV loads
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/use_types/use_types_properties.xlsx
+++ b/cea/databases/CH/archetypes/use_types/use_types_properties.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\archetypes\use_types\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\archetypes\use_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2925" windowWidth="19335" windowHeight="16455" tabRatio="785" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2930" windowWidth="19340" windowHeight="16460" tabRatio="785"/>
   </bookViews>
   <sheets>
     <sheet name="INTERNAL_LOADS" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>Ths_set_C</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>code</t>
+  </si>
+  <si>
+    <t>Ev_kW</t>
   </si>
 </sst>
 </file>
@@ -1105,30 +1108,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12" max="13" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="11.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7265625" style="1" customWidth="1"/>
+    <col min="12" max="13" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
@@ -1168,8 +1171,11 @@
       <c r="M1" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1209,8 +1215,11 @@
       <c r="M2" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1250,8 +1259,11 @@
       <c r="M3" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1291,8 +1303,11 @@
       <c r="M4" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1332,8 +1347,11 @@
       <c r="M5" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1374,8 +1392,11 @@
       <c r="M6" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
@@ -1416,8 +1437,11 @@
       <c r="M7" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1457,8 +1481,11 @@
       <c r="M8" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1498,8 +1525,11 @@
       <c r="M9" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1539,8 +1569,11 @@
       <c r="M10" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1585,8 +1618,11 @@
       <c r="M11" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1626,8 +1662,11 @@
       <c r="M12" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1667,8 +1706,11 @@
       <c r="M13" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1708,8 +1750,11 @@
       <c r="M14" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1749,8 +1794,11 @@
       <c r="M15" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -1790,8 +1838,11 @@
       <c r="M16" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
@@ -1834,8 +1885,11 @@
       <c r="M17" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
@@ -1875,8 +1929,11 @@
       <c r="M18" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -1916,8 +1973,11 @@
       <c r="M19" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>28</v>
       </c>
@@ -1955,6 +2015,9 @@
         <v>0</v>
       </c>
       <c r="M20" s="7">
+        <v>0</v>
+      </c>
+      <c r="N20" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1968,24 +2031,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
@@ -2011,7 +2074,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -2038,7 +2101,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -2065,7 +2128,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -2092,7 +2155,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
@@ -2119,7 +2182,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -2146,7 +2209,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
@@ -2173,7 +2236,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -2200,7 +2263,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -2227,7 +2290,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -2254,7 +2317,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -2281,7 +2344,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -2308,7 +2371,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -2335,7 +2398,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -2361,7 +2424,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -2387,7 +2450,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -2413,7 +2476,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
@@ -2440,7 +2503,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
@@ -2467,7 +2530,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -2494,7 +2557,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>28</v>
       </c>
@@ -2531,9 +2594,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2707,26 +2773,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2750,9 +2805,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Rename column Ev_kW to Ev_kWveh
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/use_types/use_types_properties.xlsx
+++ b/cea/databases/CH/archetypes/use_types/use_types_properties.xlsx
@@ -147,7 +147,7 @@
     <t>code</t>
   </si>
   <si>
-    <t>Ev_kW</t>
+    <t>Ev_kWveh</t>
   </si>
 </sst>
 </file>
@@ -1110,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2594,12 +2594,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2773,15 +2770,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2805,17 +2813,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>